<commit_message>
- Create FormUtil to padronize opening HDSForms - Refactoring VisitFormUtil using FormUtil to handle Editing the Form
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/visit_form.xlsx
+++ b/app/src/main/res/raw/visit_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25530" windowHeight="10020" tabRatio="500"/>
+    <workbookView windowWidth="20940" windowHeight="11595" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,30 @@
     <author>paul</author>
   </authors>
   <commentList>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>paul:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+The option is readonly, not choosable.
+Only selectable programatically, when selected make the all options read-only
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D6" authorId="0">
       <text>
         <r>
@@ -39,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="105">
   <si>
     <t>group</t>
   </si>
@@ -362,11 +386,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="26">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -396,9 +420,77 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -410,6 +502,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -417,40 +525,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -465,7 +541,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -473,44 +549,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -524,24 +562,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="SimSun"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Times New Roman"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Times New Roman"/>
+      <charset val="0"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -552,43 +587,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -600,139 +749,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -746,11 +781,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -775,21 +840,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -820,21 +870,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -846,145 +881,145 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1339,7 +1374,7 @@
   <sheetPr/>
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" topLeftCell="F1" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -1758,8 +1793,8 @@
   <sheetPr/>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="$A9:$XFD12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="5"/>
@@ -1771,7 +1806,7 @@
     <col min="5" max="5" width="13.1428571428571" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1783,6 +1818,9 @@
       </c>
       <c r="D1" t="s">
         <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1813,7 +1851,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" ht="15" customHeight="true" spans="1:4">
+    <row r="4" ht="15" customHeight="true" spans="1:5">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
@@ -1825,6 +1863,9 @@
       </c>
       <c r="D4" s="5" t="s">
         <v>74</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4">

</xml_diff>

<commit_message>
Fix Spinner Dialog on MemberFilterDialog and fix TextFilters
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/visit_form.xlsx
+++ b/app/src/main/res/raw/visit_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17670" tabRatio="500"/>
+    <workbookView windowWidth="21000" windowHeight="7575" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -394,10 +394,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -420,22 +420,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -449,17 +443,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -488,6 +491,20 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -495,33 +512,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -534,32 +528,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -571,14 +550,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="SimSun"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="SimSun"/>
-      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -602,79 +602,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -686,97 +758,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -809,6 +809,15 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
@@ -825,41 +834,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -881,6 +855,32 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -890,148 +890,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1384,7 +1384,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -1672,9 +1672,7 @@
       <c r="L11" t="b">
         <v>1</v>
       </c>
-      <c r="M11" t="b">
-        <v>1</v>
-      </c>
+      <c r="M11"/>
       <c r="N11" s="8" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
Add Dialog Input to DialogFactory
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/visit_form.xlsx
+++ b/app/src/main/res/raw/visit_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26265" windowHeight="9390" tabRatio="500"/>
+    <workbookView windowWidth="26265" windowHeight="13155" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -394,10 +394,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -431,6 +431,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -438,12 +445,97 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -458,7 +550,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -469,105 +568,6 @@
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -596,73 +596,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -674,109 +776,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -790,26 +790,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -844,17 +835,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -868,13 +864,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -890,145 +890,145 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1384,7 +1384,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -1816,7 +1816,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="I10:J10"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="5"/>

</xml_diff>

<commit_message>
- Mark all as non-visited without creating Visit Incomplete form - Hide extension details when is not enabled
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/visit_form.xlsx
+++ b/app/src/main/res/raw/visit_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12330" tabRatio="500"/>
+    <workbookView windowHeight="17730" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="112">
   <si>
     <t>group</t>
   </si>
@@ -110,6 +110,9 @@
     <t>display_style</t>
   </si>
   <si>
+    <t>hidden</t>
+  </si>
+  <si>
     <t>header</t>
   </si>
   <si>
@@ -240,6 +243,15 @@
   </si>
   <si>
     <t>${visitLocation} != 'HOME'</t>
+  </si>
+  <si>
+    <t>nonVisitedMembers</t>
+  </si>
+  <si>
+    <t>Non Visited Members</t>
+  </si>
+  <si>
+    <t>Membros não visitadosss</t>
   </si>
   <si>
     <t>collected</t>
@@ -396,8 +408,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -429,6 +441,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -436,7 +455,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -450,6 +477,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -459,31 +516,33 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF800080"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -495,9 +554,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -514,37 +572,6 @@
       <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -556,29 +583,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <sz val="9"/>
+      <name val="SimSun"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="SimSun"/>
-      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -587,7 +599,7 @@
       <charset val="0"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -596,193 +608,199 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -796,11 +814,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -809,7 +833,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -829,13 +853,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -857,6 +885,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -864,184 +903,163 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1069,10 +1087,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1388,17 +1416,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="2" max="2" width="11.1428571428571" customWidth="1"/>
     <col min="3" max="3" width="14.1428571428571" customWidth="1"/>
-    <col min="4" max="4" width="16.5047619047619" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="11.7142857142857" customWidth="1"/>
     <col min="6" max="6" width="11.0285714285714" style="10" customWidth="1"/>
     <col min="7" max="7" width="13.7142857142857" style="10" customWidth="1"/>
@@ -1410,7 +1438,7 @@
     <col min="15" max="15" width="12.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1456,22 +1484,25 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L2" t="b">
         <v>1</v>
@@ -1479,23 +1510,23 @@
       <c r="M2" t="b">
         <v>1</v>
       </c>
-      <c r="N2" s="12"/>
+      <c r="N2" s="15"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L3" t="b">
         <v>1</v>
@@ -1503,23 +1534,23 @@
       <c r="M3" t="b">
         <v>1</v>
       </c>
-      <c r="N3" s="12"/>
+      <c r="N3" s="15"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L4" t="b">
         <v>1</v>
@@ -1527,21 +1558,21 @@
       <c r="M4" t="b">
         <v>1</v>
       </c>
-      <c r="N4" s="12"/>
+      <c r="N4" s="15"/>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1"/>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L5" t="b">
         <v>1</v>
@@ -1549,43 +1580,43 @@
       <c r="M5" t="b">
         <v>1</v>
       </c>
-      <c r="N5" s="12"/>
+      <c r="N5" s="15"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1"/>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L6" t="b">
         <v>1</v>
       </c>
-      <c r="N6" s="12"/>
+      <c r="N6" s="15"/>
     </row>
     <row r="7" ht="12" customHeight="1" spans="1:14">
       <c r="A7" s="1"/>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L7" t="b">
         <v>1</v>
@@ -1593,142 +1624,148 @@
       <c r="M7" t="b">
         <v>1</v>
       </c>
-      <c r="N7" s="13" t="s">
-        <v>38</v>
+      <c r="N7" s="16" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="8" ht="16" customHeight="1" spans="4:14">
       <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" t="s">
+        <v>43</v>
+      </c>
+      <c r="L8" t="b">
+        <v>1</v>
+      </c>
+      <c r="N8" s="16" t="s">
         <v>39</v>
-      </c>
-      <c r="E8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" t="s">
-        <v>41</v>
-      </c>
-      <c r="I8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L8" t="b">
-        <v>1</v>
-      </c>
-      <c r="N8" s="13" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="9" ht="13" customHeight="1" spans="4:14">
       <c r="D9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L9" t="b">
         <v>1</v>
       </c>
-      <c r="N9" s="13" t="s">
-        <v>46</v>
+      <c r="N9" s="16" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="1"/>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L10" t="b">
         <v>1</v>
       </c>
-      <c r="N10" s="12"/>
+      <c r="N10" s="15"/>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="1"/>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L11" t="b">
         <v>1</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="1"/>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I12" t="s">
-        <v>57</v>
-      </c>
-      <c r="L12" s="11"/>
+        <v>58</v>
+      </c>
+      <c r="L12" s="14"/>
       <c r="N12" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D13" t="s">
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="11"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="I13" t="s">
-        <v>63</v>
-      </c>
-      <c r="L13" t="b">
-        <v>1</v>
-      </c>
-      <c r="M13" t="b">
-        <v>1</v>
-      </c>
-      <c r="N13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="N13" s="17"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D14" t="s">
         <v>64</v>
@@ -1748,32 +1785,53 @@
       <c r="M14" t="b">
         <v>1</v>
       </c>
-      <c r="N14" s="12"/>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="1"/>
-      <c r="F15"/>
-      <c r="G15"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
+      <c r="N14" s="15"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" t="s">
+        <v>70</v>
+      </c>
+      <c r="I15" t="s">
+        <v>71</v>
+      </c>
+      <c r="L15" t="b">
+        <v>1</v>
+      </c>
+      <c r="M15" t="b">
+        <v>1</v>
+      </c>
+      <c r="N15" s="15"/>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="1"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="1"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="1"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="1"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="1"/>
@@ -1807,6 +1865,9 @@
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.39375" footer="0.39375"/>
@@ -1838,7 +1899,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -1852,44 +1913,44 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -1897,115 +1958,115 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D7" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C8" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D8" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C9" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D9" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C10" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D10" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C11" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D11" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C12" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D12" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2033,24 +2094,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C2" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Allow upload of Visit with visitPossible=false (no extension form) - Update upload XML main tag to "xdata"
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/visit_form.xlsx
+++ b/app/src/main/res/raw/visit_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22980" windowHeight="7305" tabRatio="446" activeTab="1"/>
+    <workbookView windowWidth="27795" windowHeight="12240" tabRatio="446"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -1958,8 +1958,8 @@
   <sheetPr/>
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -2737,7 +2737,7 @@
   <sheetPr/>
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="A9" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B21" sqref="B21:B24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
- Improve display of MemberAdapter to show correctly some details - Add firlter exclude married to MemberFilterDialog - Remove some Entity relations to avoid removeAll issues
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/visit_form.xlsx
+++ b/app/src/main/res/raw/visit_form.xlsx
@@ -736,9 +736,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="28">
@@ -773,14 +773,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -788,127 +780,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -924,13 +795,142 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="9"/>
-      <name val="Times New Roman"/>
+      <name val="SimSun"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="SimSun"/>
+      <name val="Times New Roman"/>
       <charset val="134"/>
     </font>
     <font>
@@ -940,7 +940,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -961,19 +961,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.15"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="1" tint="0.5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -985,49 +1129,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1039,127 +1141,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1267,11 +1255,35 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1287,30 +1299,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1332,15 +1320,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1350,169 +1329,178 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1521,7 +1509,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1532,7 +1519,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1545,7 +1531,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1555,9 +1540,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1569,63 +1551,52 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1637,11 +1608,10 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1958,8 +1928,8 @@
   <sheetPr/>
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -1968,8 +1938,8 @@
     <col min="3" max="3" width="14.1809523809524" customWidth="1"/>
     <col min="4" max="4" width="21.8571428571429" customWidth="1"/>
     <col min="5" max="5" width="10.2857142857143" customWidth="1"/>
-    <col min="6" max="6" width="16.247619047619" style="33" customWidth="1"/>
-    <col min="7" max="7" width="12.5714285714286" style="33" customWidth="1"/>
+    <col min="6" max="6" width="15.4380952380952" style="28" customWidth="1"/>
+    <col min="7" max="7" width="12.5714285714286" style="28" customWidth="1"/>
     <col min="8" max="8" width="61" customWidth="1"/>
     <col min="9" max="9" width="55" customWidth="1"/>
     <col min="10" max="10" width="59.9904761904762" customWidth="1"/>
@@ -1998,10 +1968,10 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="28" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -2010,7 +1980,7 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="46" t="s">
+      <c r="J1" s="37" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -2025,7 +1995,7 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="33" t="s">
+      <c r="O1" s="28" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
@@ -2051,7 +2021,7 @@
       <c r="I2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="47" t="s">
+      <c r="J2" s="38" t="s">
         <v>22</v>
       </c>
       <c r="M2" t="b">
@@ -2060,7 +2030,7 @@
       <c r="N2" t="b">
         <v>1</v>
       </c>
-      <c r="O2" s="54"/>
+      <c r="O2" s="44"/>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
@@ -2078,7 +2048,7 @@
       <c r="I3" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="47" t="s">
+      <c r="J3" s="38" t="s">
         <v>26</v>
       </c>
       <c r="M3" t="b">
@@ -2087,7 +2057,7 @@
       <c r="N3" t="b">
         <v>1</v>
       </c>
-      <c r="O3" s="54"/>
+      <c r="O3" s="44"/>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="1"/>
@@ -2103,7 +2073,7 @@
       <c r="I4" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="47" t="s">
+      <c r="J4" s="38" t="s">
         <v>31</v>
       </c>
       <c r="M4" t="b">
@@ -2112,7 +2082,7 @@
       <c r="N4" t="b">
         <v>1</v>
       </c>
-      <c r="O4" s="54"/>
+      <c r="O4" s="44"/>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="1"/>
@@ -2128,7 +2098,7 @@
       <c r="I5" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="47" t="s">
+      <c r="J5" s="38" t="s">
         <v>35</v>
       </c>
       <c r="M5" t="b">
@@ -2137,7 +2107,7 @@
       <c r="N5" t="b">
         <v>1</v>
       </c>
-      <c r="O5" s="54"/>
+      <c r="O5" s="44"/>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="1"/>
@@ -2147,7 +2117,7 @@
       <c r="E6" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="33" t="s">
+      <c r="F6" s="28" t="s">
         <v>38</v>
       </c>
       <c r="H6" t="s">
@@ -2156,114 +2126,102 @@
       <c r="I6" t="s">
         <v>40</v>
       </c>
-      <c r="J6" s="47" t="s">
+      <c r="J6" s="38" t="s">
         <v>41</v>
       </c>
       <c r="M6" t="b">
         <v>1</v>
       </c>
-      <c r="O6" s="14"/>
-    </row>
-    <row r="7" s="5" customFormat="1" spans="1:17">
-      <c r="A7" s="34"/>
-      <c r="D7" s="16" t="s">
+      <c r="O6" s="12"/>
+    </row>
+    <row r="7" s="5" customFormat="1" spans="1:15">
+      <c r="A7" s="14"/>
+      <c r="D7" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="42" t="s">
+      <c r="F7" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="42"/>
-      <c r="H7" s="16" t="s">
+      <c r="G7" s="33"/>
+      <c r="H7" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="I7" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J7" s="47" t="s">
+      <c r="J7" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="N7" s="55" t="s">
+      <c r="M7" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N7" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="O7" s="56"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-    </row>
-    <row r="8" s="5" customFormat="1" spans="1:17">
-      <c r="A8" s="34"/>
-      <c r="D8" s="16" t="s">
+      <c r="O7" s="45"/>
+    </row>
+    <row r="8" s="5" customFormat="1" spans="1:15">
+      <c r="A8" s="14"/>
+      <c r="D8" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="42" t="s">
+      <c r="F8" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="G8" s="42"/>
-      <c r="H8" s="16" t="s">
+      <c r="G8" s="33"/>
+      <c r="H8" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I8" s="16" t="s">
+      <c r="I8" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="J8" s="47" t="s">
+      <c r="J8" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="N8" s="16"/>
-      <c r="O8" s="57" t="s">
+      <c r="M8" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O8" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="16"/>
-    </row>
-    <row r="9" s="28" customFormat="1" spans="1:17">
-      <c r="A9" s="35"/>
-      <c r="D9" s="28" t="s">
+    </row>
+    <row r="9" s="24" customFormat="1" spans="1:17">
+      <c r="A9" s="29"/>
+      <c r="D9" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="43" t="s">
+      <c r="F9" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="43"/>
-      <c r="H9" s="28" t="s">
+      <c r="G9" s="34"/>
+      <c r="H9" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="28" t="s">
+      <c r="I9" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="J9" s="48" t="s">
+      <c r="J9" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="N9" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="O9" s="58" t="s">
+      <c r="M9" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="N9" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="O9" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="P9" s="28"/>
-      <c r="Q9" s="28" t="b">
+      <c r="Q9" s="24" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2275,7 +2233,7 @@
       <c r="E10" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="33" t="s">
+      <c r="F10" s="28" t="s">
         <v>43</v>
       </c>
       <c r="H10" t="s">
@@ -2284,7 +2242,7 @@
       <c r="I10" t="s">
         <v>59</v>
       </c>
-      <c r="J10" s="47" t="s">
+      <c r="J10" s="38" t="s">
         <v>60</v>
       </c>
       <c r="M10" t="b">
@@ -2293,7 +2251,7 @@
       <c r="N10" t="b">
         <v>1</v>
       </c>
-      <c r="O10" s="14" t="s">
+      <c r="O10" s="12" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2305,7 +2263,7 @@
       <c r="E11" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="33" t="s">
+      <c r="F11" s="28" t="s">
         <v>63</v>
       </c>
       <c r="H11" t="s">
@@ -2314,13 +2272,13 @@
       <c r="I11" t="s">
         <v>65</v>
       </c>
-      <c r="J11" s="47" t="s">
+      <c r="J11" s="38" t="s">
         <v>66</v>
       </c>
       <c r="M11" t="b">
         <v>1</v>
       </c>
-      <c r="O11" s="14" t="s">
+      <c r="O11" s="12" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2338,7 +2296,7 @@
       <c r="I12" t="s">
         <v>70</v>
       </c>
-      <c r="J12" s="47" t="s">
+      <c r="J12" s="38" t="s">
         <v>71</v>
       </c>
       <c r="M12" t="b">
@@ -2347,7 +2305,7 @@
       <c r="N12" t="b">
         <v>1</v>
       </c>
-      <c r="O12" s="59" t="s">
+      <c r="O12" s="48" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2365,16 +2323,16 @@
       <c r="I13" t="s">
         <v>75</v>
       </c>
-      <c r="J13" s="47" t="s">
+      <c r="J13" s="38" t="s">
         <v>76</v>
       </c>
       <c r="M13" t="b">
         <v>1</v>
       </c>
-      <c r="N13" s="60" t="s">
+      <c r="N13" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="O13" s="61" t="s">
+      <c r="O13" s="50" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2385,7 +2343,7 @@
       <c r="E14" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="33" t="s">
+      <c r="F14" s="28" t="s">
         <v>43</v>
       </c>
       <c r="H14" t="s">
@@ -2394,13 +2352,13 @@
       <c r="I14" t="s">
         <v>81</v>
       </c>
-      <c r="J14" s="47" t="s">
+      <c r="J14" s="38" t="s">
         <v>82</v>
       </c>
       <c r="M14" t="b">
         <v>1</v>
       </c>
-      <c r="O14" s="59" t="s">
+      <c r="O14" s="48" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2417,13 +2375,13 @@
       <c r="I15" t="s">
         <v>85</v>
       </c>
-      <c r="J15" s="47" t="s">
+      <c r="J15" s="38" t="s">
         <v>86</v>
       </c>
       <c r="M15" t="b">
         <v>1</v>
       </c>
-      <c r="O15" s="59" t="s">
+      <c r="O15" s="48" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2435,7 +2393,7 @@
       <c r="E16" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="33" t="s">
+      <c r="F16" s="28" t="s">
         <v>89</v>
       </c>
       <c r="H16" t="s">
@@ -2444,13 +2402,13 @@
       <c r="I16" t="s">
         <v>91</v>
       </c>
-      <c r="J16" s="47" t="s">
+      <c r="J16" s="38" t="s">
         <v>92</v>
       </c>
       <c r="M16" t="b">
         <v>1</v>
       </c>
-      <c r="O16" s="14" t="s">
+      <c r="O16" s="12" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2468,13 +2426,13 @@
       <c r="I17" t="s">
         <v>96</v>
       </c>
-      <c r="J17" s="47" t="s">
+      <c r="J17" s="38" t="s">
         <v>97</v>
       </c>
       <c r="M17" t="b">
         <v>1</v>
       </c>
-      <c r="O17" s="14" t="s">
+      <c r="O17" s="12" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2492,178 +2450,152 @@
       <c r="I18" t="s">
         <v>101</v>
       </c>
-      <c r="J18" s="49" t="s">
+      <c r="J18" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="M18" s="62"/>
-      <c r="O18" s="14" t="s">
+      <c r="M18" s="5"/>
+      <c r="O18" s="12" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="19" s="29" customFormat="1" spans="1:17">
-      <c r="A19" s="36"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37" t="s">
+    <row r="19" s="25" customFormat="1" spans="1:17">
+      <c r="A19" s="30"/>
+      <c r="D19" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="E19" s="37" t="s">
+      <c r="E19" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="44"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="37" t="s">
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="I19" s="37" t="s">
+      <c r="I19" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="J19" s="50" t="s">
+      <c r="J19" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="K19" s="37"/>
-      <c r="L19" s="37"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="O19" s="63"/>
-      <c r="P19" s="37"/>
-      <c r="Q19" s="37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" s="30" customFormat="1" spans="1:17">
-      <c r="A20" s="38" t="s">
+      <c r="N19" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="O19" s="51"/>
+      <c r="Q19" s="25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" s="26" customFormat="1" spans="1:15">
+      <c r="A20" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="B20" s="39"/>
-      <c r="C20" s="39"/>
-      <c r="D20" s="39" t="s">
+      <c r="D20" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="E20" s="39" t="s">
+      <c r="E20" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="F20" s="45"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="39" t="s">
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="I20" s="39" t="s">
+      <c r="I20" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="J20" s="51" t="s">
+      <c r="J20" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="K20" s="39"/>
-      <c r="L20" s="39"/>
-      <c r="M20" s="39" t="b">
-        <v>1</v>
-      </c>
-      <c r="N20" s="39" t="b">
-        <v>1</v>
-      </c>
-      <c r="O20" s="64"/>
-      <c r="P20" s="39"/>
-      <c r="Q20" s="39"/>
-    </row>
-    <row r="21" s="28" customFormat="1" spans="1:15">
-      <c r="A21" s="38" t="s">
+      <c r="M20" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="N20" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="O20" s="52"/>
+    </row>
+    <row r="21" s="24" customFormat="1" spans="1:15">
+      <c r="A21" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="E21" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="28" t="s">
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="I21" s="28" t="s">
+      <c r="I21" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="J21" s="48" t="s">
+      <c r="J21" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="M21" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="N21" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="O21" s="52"/>
-    </row>
-    <row r="22" s="31" customFormat="1" spans="1:17">
-      <c r="A22" s="38" t="s">
+      <c r="M21" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="N21" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="O21" s="42"/>
+    </row>
+    <row r="22" s="24" customFormat="1" spans="1:17">
+      <c r="A22" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="E22" s="28" t="s">
+      <c r="E22" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28" t="s">
+      <c r="H22" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="I22" s="28" t="s">
+      <c r="I22" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="J22" s="48" t="s">
+      <c r="J22" s="39" t="s">
         <v>121</v>
       </c>
-      <c r="K22" s="52"/>
-      <c r="L22" s="52"/>
-      <c r="M22" s="28"/>
-      <c r="N22" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="O22" s="28"/>
-      <c r="P22" s="28"/>
-      <c r="Q22" s="28" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" s="32" customFormat="1" spans="1:17">
-      <c r="A23" s="40" t="s">
+      <c r="K22" s="42"/>
+      <c r="L22" s="42"/>
+      <c r="N22" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" s="27" customFormat="1" spans="1:17">
+      <c r="A23" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41" t="s">
+      <c r="D23" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="E23" s="41" t="s">
+      <c r="E23" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="41"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="41" t="s">
+      <c r="H23" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="I23" s="41" t="s">
+      <c r="I23" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="J23" s="48" t="s">
+      <c r="J23" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="K23" s="53"/>
-      <c r="L23" s="53"/>
-      <c r="M23" s="41"/>
-      <c r="N23" s="41" t="b">
-        <v>1</v>
-      </c>
-      <c r="O23" s="41"/>
-      <c r="P23" s="41"/>
-      <c r="Q23" s="41" t="b">
+      <c r="K23" s="43"/>
+      <c r="L23" s="43"/>
+      <c r="N23" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="27" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2671,23 +2603,23 @@
       <c r="A24" s="1"/>
       <c r="F24"/>
       <c r="G24"/>
-      <c r="K24" s="54"/>
-      <c r="L24" s="54"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="44"/>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="1"/>
-      <c r="K25" s="54"/>
-      <c r="L25" s="54"/>
+      <c r="K25" s="44"/>
+      <c r="L25" s="44"/>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="1"/>
-      <c r="K26" s="54"/>
-      <c r="L26" s="54"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="44"/>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="1"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="1"/>
@@ -2764,7 +2696,7 @@
       <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="18" t="s">
         <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -2772,53 +2704,53 @@
       </c>
     </row>
     <row r="2" s="3" customFormat="1" spans="1:5">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="19" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="3" s="3" customFormat="1" ht="15" customHeight="1" spans="1:5">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="20" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="4" s="3" customFormat="1" ht="15" customHeight="1" spans="1:6">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="21" t="s">
         <v>136</v>
       </c>
       <c r="F4" s="3" t="b">
@@ -2826,36 +2758,36 @@
       </c>
     </row>
     <row r="5" s="3" customFormat="1" spans="1:5">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="19" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="6" s="3" customFormat="1" spans="1:5">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="22" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2863,7 +2795,7 @@
       <c r="A7" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="12" t="s">
         <v>145</v>
       </c>
       <c r="C7" t="s">
@@ -2872,7 +2804,7 @@
       <c r="D7" t="s">
         <v>147</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="18" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2880,7 +2812,7 @@
       <c r="A8" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="12" t="s">
         <v>149</v>
       </c>
       <c r="C8" t="s">
@@ -2889,7 +2821,7 @@
       <c r="D8" t="s">
         <v>151</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="18" t="s">
         <v>152</v>
       </c>
     </row>
@@ -2897,7 +2829,7 @@
       <c r="A9" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="13" t="s">
         <v>153</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -2906,7 +2838,7 @@
       <c r="D9" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="23" t="s">
         <v>156</v>
       </c>
     </row>
@@ -2914,7 +2846,7 @@
       <c r="A10" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="13" t="s">
         <v>157</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -2923,7 +2855,7 @@
       <c r="D10" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="23" t="s">
         <v>160</v>
       </c>
     </row>
@@ -2931,7 +2863,7 @@
       <c r="A11" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="13" t="s">
         <v>161</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -2940,7 +2872,7 @@
       <c r="D11" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="23" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2948,7 +2880,7 @@
       <c r="A12" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="13" t="s">
         <v>165</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -2957,167 +2889,160 @@
       <c r="D12" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="23" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="13" s="5" customFormat="1" spans="1:6">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="F13" s="16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" s="5" customFormat="1" spans="1:6">
-      <c r="A14" s="16" t="s">
+      <c r="F13" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" s="5" customFormat="1" spans="1:5">
+      <c r="A14" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="F14" s="16"/>
-    </row>
-    <row r="15" s="5" customFormat="1" spans="1:6">
-      <c r="A15" s="16" t="s">
+    </row>
+    <row r="15" s="5" customFormat="1" spans="1:5">
+      <c r="A15" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="F15" s="16"/>
-    </row>
-    <row r="16" s="5" customFormat="1" spans="1:6">
-      <c r="A16" s="16" t="s">
+    </row>
+    <row r="16" s="5" customFormat="1" spans="1:5">
+      <c r="A16" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="F16" s="16"/>
-    </row>
-    <row r="17" s="5" customFormat="1" spans="1:6">
-      <c r="A17" s="16" t="s">
+    </row>
+    <row r="17" s="5" customFormat="1" spans="1:5">
+      <c r="A17" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="F17" s="16"/>
-    </row>
-    <row r="18" s="5" customFormat="1" spans="1:6">
-      <c r="A18" s="16" t="s">
+    </row>
+    <row r="18" s="5" customFormat="1" spans="1:5">
+      <c r="A18" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="D18" s="18" t="s">
+      <c r="D18" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="F18" s="16"/>
-    </row>
-    <row r="19" s="5" customFormat="1" spans="1:6">
-      <c r="A19" s="16" t="s">
+    </row>
+    <row r="19" s="5" customFormat="1" spans="1:5">
+      <c r="A19" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="F19" s="16"/>
-    </row>
-    <row r="20" s="5" customFormat="1" spans="1:6">
-      <c r="A20" s="16" t="s">
+    </row>
+    <row r="20" s="5" customFormat="1" spans="1:5">
+      <c r="A20" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="F20" s="16"/>
     </row>
     <row r="21" s="4" customFormat="1" spans="1:5">
       <c r="A21" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="13" t="s">
         <v>200</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="16" t="s">
         <v>202</v>
       </c>
       <c r="E21" s="4" t="s">
@@ -3128,55 +3053,55 @@
       <c r="A22" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="13" t="s">
         <v>204</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D22" s="17" t="s">
         <v>206</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="23" s="6" customFormat="1" spans="1:5">
-      <c r="A23" s="6" t="s">
+    <row r="23" s="4" customFormat="1" spans="1:5">
+      <c r="A23" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="4" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="24" s="6" customFormat="1" spans="1:5">
-      <c r="A24" s="6" t="s">
+    <row r="24" s="4" customFormat="1" spans="1:5">
+      <c r="A24" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="4" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="25" s="6" customFormat="1" spans="2:2">
-      <c r="B25" s="21"/>
+    <row r="25" s="4" customFormat="1" spans="2:2">
+      <c r="B25" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update commons-io library TO 2.16.1
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/visit_form.xlsx
+++ b/app/src/main/res/raw/visit_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22725" windowHeight="8490" tabRatio="446"/>
+    <workbookView windowWidth="18045" windowHeight="6780" tabRatio="446"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="223">
   <si>
     <t>group</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>roundNumber</t>
+  </si>
+  <si>
+    <t>integer</t>
   </si>
   <si>
     <t>1.3. Round Number</t>
@@ -737,9 +740,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -773,18 +776,25 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Arial"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -803,21 +813,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -826,23 +821,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -864,23 +851,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -894,16 +866,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -916,9 +904,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -967,6 +970,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -979,13 +988,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -997,157 +1126,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1255,6 +1258,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1266,6 +1280,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1285,20 +1308,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1320,26 +1340,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1347,156 +1350,156 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1928,8 +1931,8 @@
   <sheetPr/>
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -2090,16 +2093,16 @@
         <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="H5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J5" s="38" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M5" t="b">
         <v>1</v>
@@ -2112,22 +2115,22 @@
     <row r="6" spans="1:15">
       <c r="A6" s="1"/>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J6" s="38" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M6" t="b">
         <v>1</v>
@@ -2137,80 +2140,80 @@
     <row r="7" s="5" customFormat="1" spans="1:15">
       <c r="A7" s="14"/>
       <c r="D7" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G7" s="33"/>
       <c r="H7" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J7" s="38" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M7" s="5" t="b">
         <v>1</v>
       </c>
       <c r="N7" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="O7" s="45"/>
     </row>
     <row r="8" s="5" customFormat="1" spans="1:15">
       <c r="A8" s="14"/>
       <c r="D8" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F8" s="33" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G8" s="33"/>
       <c r="H8" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J8" s="38" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="M8" s="5" t="b">
         <v>1</v>
       </c>
       <c r="O8" s="46" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" s="24" customFormat="1" spans="1:17">
       <c r="A9" s="29"/>
       <c r="D9" s="24" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F9" s="34" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G9" s="34"/>
       <c r="H9" s="24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J9" s="39" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M9" s="24" t="b">
         <v>1</v>
@@ -2219,7 +2222,7 @@
         <v>1</v>
       </c>
       <c r="O9" s="47" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q9" s="24" t="b">
         <v>1</v>
@@ -2228,22 +2231,22 @@
     <row r="10" spans="1:15">
       <c r="A10" s="1"/>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J10" s="38" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="M10" t="b">
         <v>1</v>
@@ -2252,52 +2255,52 @@
         <v>1</v>
       </c>
       <c r="O10" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="1"/>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J11" s="38" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M11" t="b">
         <v>1</v>
       </c>
       <c r="O11" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" ht="12" customHeight="1" spans="1:15">
       <c r="A12" s="1"/>
       <c r="D12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E12" t="s">
         <v>19</v>
       </c>
       <c r="H12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J12" s="38" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="M12" t="b">
         <v>1</v>
@@ -2306,162 +2309,162 @@
         <v>1</v>
       </c>
       <c r="O12" s="48" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" ht="12" customHeight="1" spans="1:15">
       <c r="A13" s="1"/>
       <c r="D13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E13" t="s">
         <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I13" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="J13" s="38" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M13" t="b">
         <v>1</v>
       </c>
       <c r="N13" s="49" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="O13" s="50" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" ht="13" customHeight="1" spans="4:15">
       <c r="D14" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F14" s="28" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J14" s="38" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="M14" t="b">
         <v>1</v>
       </c>
       <c r="O14" s="48" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" ht="13" customHeight="1" spans="4:15">
       <c r="D15" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E15" t="s">
         <v>19</v>
       </c>
       <c r="H15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I15" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J15" s="38" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M15" t="b">
         <v>1</v>
       </c>
       <c r="O15" s="48" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="1"/>
       <c r="D16" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F16" s="28" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H16" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I16" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J16" s="38" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="M16" t="b">
         <v>1</v>
       </c>
       <c r="O16" s="12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" s="1"/>
       <c r="D17" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E17" t="s">
         <v>19</v>
       </c>
       <c r="H17" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J17" s="38" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="M17" t="b">
         <v>1</v>
       </c>
       <c r="O17" s="12" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="1"/>
       <c r="D18" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E18" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I18" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J18" s="40" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M18" s="5"/>
       <c r="O18" s="12" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" s="25" customFormat="1" spans="1:17">
       <c r="A19" s="30"/>
       <c r="D19" s="25" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E19" s="25" t="s">
         <v>19</v>
@@ -2469,13 +2472,13 @@
       <c r="F19" s="35"/>
       <c r="G19" s="35"/>
       <c r="H19" s="25" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I19" s="25" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J19" s="25" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="N19" s="25" t="b">
         <v>1</v>
@@ -2487,24 +2490,24 @@
     </row>
     <row r="20" s="26" customFormat="1" spans="1:15">
       <c r="A20" s="31" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F20" s="36"/>
       <c r="G20" s="36"/>
       <c r="H20" s="26" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I20" s="26" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J20" s="41" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="M20" s="26" t="b">
         <v>1</v>
@@ -2516,24 +2519,24 @@
     </row>
     <row r="21" s="24" customFormat="1" spans="1:15">
       <c r="A21" s="31" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F21" s="34"/>
       <c r="G21" s="34"/>
       <c r="H21" s="24" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I21" s="24" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J21" s="39" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="M21" s="24" t="b">
         <v>1</v>
@@ -2545,22 +2548,22 @@
     </row>
     <row r="22" s="24" customFormat="1" spans="1:17">
       <c r="A22" s="31" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H22" s="24" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I22" s="24" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J22" s="39" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="K22" s="42"/>
       <c r="L22" s="42"/>
@@ -2573,22 +2576,22 @@
     </row>
     <row r="23" s="27" customFormat="1" spans="1:17">
       <c r="A23" s="32" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D23" s="27" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E23" s="27" t="s">
         <v>19</v>
       </c>
       <c r="H23" s="27" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I23" s="27" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J23" s="39" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="K23" s="43"/>
       <c r="L23" s="43"/>
@@ -2688,7 +2691,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -2705,53 +2708,53 @@
     </row>
     <row r="2" s="3" customFormat="1" spans="1:5">
       <c r="A2" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" s="3" customFormat="1" ht="15" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" s="3" customFormat="1" ht="15" customHeight="1" spans="1:6">
       <c r="A4" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F4" s="3" t="b">
         <v>1</v>
@@ -2759,155 +2762,155 @@
     </row>
     <row r="5" s="3" customFormat="1" spans="1:5">
       <c r="A5" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" s="3" customFormat="1" spans="1:5">
       <c r="A6" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C7" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" s="4" customFormat="1" spans="1:5">
       <c r="A9" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" s="4" customFormat="1" spans="1:5">
       <c r="A10" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" s="4" customFormat="1" spans="1:5">
       <c r="A11" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" s="4" customFormat="1" spans="1:5">
       <c r="A12" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="13" s="5" customFormat="1" spans="1:6">
       <c r="A13" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F13" s="5" t="b">
         <v>1</v>
@@ -2915,189 +2918,189 @@
     </row>
     <row r="14" s="5" customFormat="1" spans="1:5">
       <c r="A14" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" s="5" customFormat="1" spans="1:5">
       <c r="A15" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" s="5" customFormat="1" spans="1:5">
       <c r="A16" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17" s="5" customFormat="1" spans="1:5">
       <c r="A17" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" s="5" customFormat="1" spans="1:5">
       <c r="A18" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="19" s="5" customFormat="1" spans="1:5">
       <c r="A19" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" s="5" customFormat="1" spans="1:5">
       <c r="A20" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" s="4" customFormat="1" spans="1:5">
       <c r="A21" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="22" s="4" customFormat="1" spans="1:5">
       <c r="A22" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" s="4" customFormat="1" spans="1:5">
       <c r="A23" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="24" s="4" customFormat="1" spans="1:5">
       <c r="A24" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="25" s="4" customFormat="1" spans="2:2">
@@ -3128,30 +3131,30 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Add support for 'GPS Required' parameter to enable enforcement of GPS capture on all visits - Update Visit Form constraints and add visitReasonOther, otherNotPossibleReason to capture other reasons for a visit
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/visit_form.xlsx
+++ b/app/src/main/res/raw/visit_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18045" windowHeight="6780" tabRatio="446"/>
+    <workbookView windowWidth="27795" windowHeight="12195" tabRatio="446"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,38 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>paul</author>
+  </authors>
+  <commentList>
+    <comment ref="M22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>paul:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+Track this from the Sites, if they want it to be optional or not.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>paul</author>
@@ -63,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="238">
   <si>
     <t>group</t>
   </si>
@@ -176,12 +208,30 @@
     <t>1.3. Numéro du Tour</t>
   </si>
   <si>
+    <t>respondentExists</t>
+  </si>
+  <si>
+    <t>select</t>
+  </si>
+  <si>
+    <t>yes_no</t>
+  </si>
+  <si>
+    <t>1.X. Respondent Exists (hidden)</t>
+  </si>
+  <si>
+    <t>1.X Respondent Exists (hidden)</t>
+  </si>
+  <si>
+    <t>respondentNotResident</t>
+  </si>
+  <si>
+    <t>1.X. Respondent not a resident of this Household (hidden)</t>
+  </si>
+  <si>
     <t>visitReason</t>
   </si>
   <si>
-    <t>select</t>
-  </si>
-  <si>
     <t>reasons</t>
   </si>
   <si>
@@ -194,12 +244,24 @@
     <t>1.4. Motif de la Visite</t>
   </si>
   <si>
+    <t>visitReasonOther</t>
+  </si>
+  <si>
+    <t>1.4.1. Specify the reason for visit?</t>
+  </si>
+  <si>
+    <t>1.4.1. Especifique o motivo da visita?</t>
+  </si>
+  <si>
+    <t>1.4.1. Spécifiez la raison de la visite ?</t>
+  </si>
+  <si>
+    <t>${visitReason} = 'OTHER'</t>
+  </si>
+  <si>
     <t>visitPossible</t>
   </si>
   <si>
-    <t>yes_no</t>
-  </si>
-  <si>
     <t>2.1. Is it possible to perform a visit to this Household?</t>
   </si>
   <si>
@@ -230,13 +292,19 @@
     <t>${visitPossible} = 'false'</t>
   </si>
   <si>
-    <t>respondentExists</t>
-  </si>
-  <si>
-    <t>2.2.0. Respondent Exists (hidden)</t>
-  </si>
-  <si>
-    <t>${visitNotPossibleReason}!='NO_RESPONDENT' and ${visitNotPossibleReason}!='REFUSE'</t>
+    <t>otherNotPossibleReason</t>
+  </si>
+  <si>
+    <t>2.1.2. Specify the reason for not being able to perform the visit?</t>
+  </si>
+  <si>
+    <t>2.1.2. Especifique o motivo de não ser possível realizar a visita?</t>
+  </si>
+  <si>
+    <t>2.1.2. Précisez la raison pour laquelle il n'est pas possible d'effectuer la visite?</t>
+  </si>
+  <si>
+    <t>${visitNotPossibleReason} = 'OTHER'</t>
   </si>
   <si>
     <t>respondentResident</t>
@@ -251,7 +319,7 @@
     <t>2.2. Le répondant est-il résident de ce Ménage?</t>
   </si>
   <si>
-    <t>${visitReason} != 'NEW_HOUSE' and (${respondentExists}='true' or ${respondentExists}='false')</t>
+    <t>(${visitReason} != 'NEW_HOUSE') and (${respondentExists} = 'true' or ${respondentExists} = 'false') and (${visitNotPossibleReason} != 'NO_RESPONDENT') and (${visitNotPossibleReason} != 'REFUSE')</t>
   </si>
   <si>
     <t>respondentRelationship</t>
@@ -284,7 +352,7 @@
     <t>2.2. Code du répondant</t>
   </si>
   <si>
-    <t>${visitReason} != 'NEW_HOUSE' and ${respondentExists} = 'true'</t>
+    <t>${visitReason} != 'NEW_HOUSE' and ${respondentExists} = 'true' and (${visitNotPossibleReason} != 'NO_RESPONDENT') and (${visitNotPossibleReason} != 'REFUSE')</t>
   </si>
   <si>
     <t>respondentName</t>
@@ -302,7 +370,7 @@
     <t>${respondentExists} = 'true'</t>
   </si>
   <si>
-    <t>${visitReason} != 'NEW_HOUSE' and (${respondentExists} = 'true' or ${respondentExists} = 'false')</t>
+    <t>${visitReason} != 'NEW_HOUSE' and (${respondentExists} = 'true' or ${respondentExists} = 'false') and (${visitNotPossibleReason} != 'NO_RESPONDENT') and (${visitNotPossibleReason} != 'REFUSE')</t>
   </si>
   <si>
     <t>hasInterpreter</t>
@@ -365,6 +433,12 @@
     <t>${visitLocation} = 'OTHERPLACE'</t>
   </si>
   <si>
+    <t>gpsRequired</t>
+  </si>
+  <si>
+    <t>2.7.0. Is GPS Required (hidden)</t>
+  </si>
+  <si>
     <t>gps</t>
   </si>
   <si>
@@ -377,7 +451,23 @@
     <t>2.5. Enregistrement des coordonnées GPS</t>
   </si>
   <si>
-    <t>${visitPossible} = 'true' and ${visitLocation} != 'HOME'</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>(${visitPossible} = 'true' and ${visitLocation} != 'HOME') or</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> (${gpsRequired} = 'true')</t>
+    </r>
   </si>
   <si>
     <t>nonVisitedMembers</t>
@@ -645,6 +735,9 @@
   </si>
   <si>
     <t>Pas d'informateur</t>
+  </si>
+  <si>
+    <t>${respondentExists} = 'true' or ${respondentNotResident} = 'true'</t>
   </si>
   <si>
     <t>REFUSE</t>
@@ -741,10 +834,10 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="31">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -776,25 +869,16 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="10"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -813,23 +897,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -844,6 +913,14 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Arial"/>
@@ -851,8 +928,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -861,6 +947,20 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -881,17 +981,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -899,6 +990,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -914,14 +1013,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -932,18 +1031,29 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Times New Roman"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Times New Roman"/>
+      <charset val="0"/>
+    </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -970,7 +1080,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="0" tint="-0.5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -982,7 +1116,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -994,25 +1206,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1024,79 +1254,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1108,49 +1266,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1258,17 +1374,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1293,6 +1398,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1304,21 +1418,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1347,163 +1446,180 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1554,14 +1670,19 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1573,35 +1694,42 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1610,6 +1738,13 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1929,10 +2064,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Q39"/>
+  <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <pane xSplit="7" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection/>
+      <selection pane="topRight" activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -1941,16 +2078,16 @@
     <col min="3" max="3" width="14.1809523809524" customWidth="1"/>
     <col min="4" max="4" width="21.8571428571429" customWidth="1"/>
     <col min="5" max="5" width="10.2857142857143" customWidth="1"/>
-    <col min="6" max="6" width="15.4380952380952" style="28" customWidth="1"/>
-    <col min="7" max="7" width="12.5714285714286" style="28" customWidth="1"/>
+    <col min="6" max="6" width="15.4380952380952" style="30" customWidth="1"/>
+    <col min="7" max="7" width="12.5714285714286" style="30" customWidth="1"/>
     <col min="8" max="8" width="61" customWidth="1"/>
     <col min="9" max="9" width="55" customWidth="1"/>
     <col min="10" max="10" width="59.9904761904762" customWidth="1"/>
     <col min="11" max="11" width="12.8571428571429" customWidth="1"/>
     <col min="12" max="12" width="10.4285714285714" customWidth="1"/>
-    <col min="13" max="13" width="9.26666666666667" customWidth="1"/>
+    <col min="13" max="13" width="21.2857142857143" customWidth="1"/>
     <col min="14" max="14" width="30.4285714285714" customWidth="1"/>
-    <col min="15" max="15" width="79.8571428571429" customWidth="1"/>
+    <col min="15" max="15" width="106.066666666667" customWidth="1"/>
     <col min="16" max="16" width="12.7142857142857" customWidth="1"/>
     <col min="17" max="17" width="7" customWidth="1"/>
   </cols>
@@ -1971,10 +2108,10 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="30" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -1983,7 +2120,7 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="J1" s="42" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -1998,7 +2135,7 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="O1" s="30" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
@@ -2024,7 +2161,7 @@
       <c r="I2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="38" t="s">
+      <c r="J2" s="43" t="s">
         <v>22</v>
       </c>
       <c r="M2" t="b">
@@ -2033,7 +2170,7 @@
       <c r="N2" t="b">
         <v>1</v>
       </c>
-      <c r="O2" s="44"/>
+      <c r="O2" s="50"/>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
@@ -2051,7 +2188,7 @@
       <c r="I3" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="38" t="s">
+      <c r="J3" s="43" t="s">
         <v>26</v>
       </c>
       <c r="M3" t="b">
@@ -2060,7 +2197,7 @@
       <c r="N3" t="b">
         <v>1</v>
       </c>
-      <c r="O3" s="44"/>
+      <c r="O3" s="50"/>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="1"/>
@@ -2076,7 +2213,7 @@
       <c r="I4" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="38" t="s">
+      <c r="J4" s="43" t="s">
         <v>31</v>
       </c>
       <c r="M4" t="b">
@@ -2085,7 +2222,7 @@
       <c r="N4" t="b">
         <v>1</v>
       </c>
-      <c r="O4" s="44"/>
+      <c r="O4" s="50"/>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="1"/>
@@ -2101,7 +2238,7 @@
       <c r="I5" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="38" t="s">
+      <c r="J5" s="43" t="s">
         <v>36</v>
       </c>
       <c r="M5" t="b">
@@ -2110,531 +2247,635 @@
       <c r="N5" t="b">
         <v>1</v>
       </c>
-      <c r="O5" s="44"/>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="1"/>
-      <c r="D6" t="s">
+      <c r="O5" s="50"/>
+    </row>
+    <row r="6" s="24" customFormat="1" spans="1:17">
+      <c r="A6" s="31"/>
+      <c r="D6" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="28" t="s">
+      <c r="F6" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="H6" t="s">
+      <c r="G6" s="36"/>
+      <c r="H6" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="38" t="s">
+      <c r="M6" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="N6" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="O6" s="51"/>
+      <c r="Q6" s="24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" s="24" customFormat="1" spans="1:17">
+      <c r="A7" s="31"/>
+      <c r="D7" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="M6" t="b">
-        <v>1</v>
-      </c>
-      <c r="O6" s="12"/>
-    </row>
-    <row r="7" s="5" customFormat="1" spans="1:15">
-      <c r="A7" s="14"/>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="36"/>
+      <c r="H7" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="I7" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="N7" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="O7" s="51"/>
+      <c r="Q7" s="24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="1"/>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="33"/>
-      <c r="H7" s="5" t="s">
+      <c r="F8" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="H8" t="s">
         <v>46</v>
       </c>
-      <c r="J7" s="38" t="s">
+      <c r="I8" t="s">
         <v>47</v>
       </c>
-      <c r="M7" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="N7" s="14" t="s">
+      <c r="J8" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="O7" s="45"/>
-    </row>
-    <row r="8" s="5" customFormat="1" spans="1:15">
-      <c r="A8" s="14"/>
-      <c r="D8" s="5" t="s">
+      <c r="M8" t="b">
+        <v>1</v>
+      </c>
+      <c r="O8" s="12"/>
+    </row>
+    <row r="9" customFormat="1" spans="1:15">
+      <c r="A9" s="1"/>
+      <c r="D9" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="M9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O9" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" s="5" customFormat="1" spans="1:15">
+      <c r="A10" s="14"/>
+      <c r="D10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8" s="33"/>
-      <c r="H8" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="J8" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="M8" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="O8" s="46" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" s="24" customFormat="1" spans="1:17">
-      <c r="A9" s="29"/>
-      <c r="D9" s="24" t="s">
+      <c r="F10" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="37"/>
+      <c r="H10" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="I10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="M10" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N10" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="O10" s="52"/>
+    </row>
+    <row r="11" s="5" customFormat="1" spans="1:15">
+      <c r="A11" s="14"/>
+      <c r="D11" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="34"/>
-      <c r="H9" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="J9" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="M9" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="N9" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="O9" s="47" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q9" s="24" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" s="1"/>
-      <c r="D10" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="H10" t="s">
-        <v>59</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="F11" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="J10" s="38" t="s">
+      <c r="G11" s="37"/>
+      <c r="H11" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="M10" t="b">
-        <v>1</v>
-      </c>
-      <c r="N10" t="b">
-        <v>1</v>
-      </c>
-      <c r="O10" s="12" t="s">
+      <c r="I11" s="5" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" s="1"/>
-      <c r="D11" t="s">
+      <c r="J11" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="E11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="28" t="s">
+      <c r="M11" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O11" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="H11" t="s">
+    </row>
+    <row r="12" s="5" customFormat="1" spans="1:15">
+      <c r="A12" s="14"/>
+      <c r="D12" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="I11" t="s">
+      <c r="E12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="J11" s="38" t="s">
+      <c r="I12" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="M11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O11" s="12" t="s">
+      <c r="J12" s="43" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="12" ht="12" customHeight="1" spans="1:15">
-      <c r="A12" s="1"/>
-      <c r="D12" t="s">
+      <c r="M12" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O12" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="E12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" t="s">
-        <v>70</v>
-      </c>
-      <c r="I12" t="s">
-        <v>71</v>
-      </c>
-      <c r="J12" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="M12" t="b">
-        <v>1</v>
-      </c>
-      <c r="N12" t="b">
-        <v>1</v>
-      </c>
-      <c r="O12" s="48" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" ht="12" customHeight="1" spans="1:15">
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="1"/>
       <c r="D13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" t="s">
+        <v>71</v>
+      </c>
+      <c r="I13" t="s">
+        <v>72</v>
+      </c>
+      <c r="J13" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="M13" t="b">
+        <v>1</v>
+      </c>
+      <c r="N13" t="b">
+        <v>1</v>
+      </c>
+      <c r="O13" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="E13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13" t="s">
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="1"/>
+      <c r="D14" t="s">
         <v>75</v>
-      </c>
-      <c r="I13" t="s">
-        <v>76</v>
-      </c>
-      <c r="J13" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="M13" t="b">
-        <v>1</v>
-      </c>
-      <c r="N13" s="49" t="s">
-        <v>78</v>
-      </c>
-      <c r="O13" s="50" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" ht="13" customHeight="1" spans="4:15">
-      <c r="D14" t="s">
-        <v>80</v>
       </c>
       <c r="E14" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="28" t="s">
-        <v>44</v>
+      <c r="F14" s="30" t="s">
+        <v>76</v>
       </c>
       <c r="H14" t="s">
+        <v>77</v>
+      </c>
+      <c r="I14" t="s">
+        <v>78</v>
+      </c>
+      <c r="J14" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="M14" t="b">
+        <v>1</v>
+      </c>
+      <c r="O14" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" ht="12" customHeight="1" spans="1:15">
+      <c r="A15" s="1"/>
+      <c r="D15" t="s">
         <v>81</v>
-      </c>
-      <c r="I14" t="s">
-        <v>82</v>
-      </c>
-      <c r="J14" s="38" t="s">
-        <v>83</v>
-      </c>
-      <c r="M14" t="b">
-        <v>1</v>
-      </c>
-      <c r="O14" s="48" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" ht="13" customHeight="1" spans="4:15">
-      <c r="D15" t="s">
-        <v>84</v>
       </c>
       <c r="E15" t="s">
         <v>19</v>
       </c>
       <c r="H15" t="s">
+        <v>82</v>
+      </c>
+      <c r="I15" t="s">
+        <v>83</v>
+      </c>
+      <c r="J15" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="M15" t="b">
+        <v>1</v>
+      </c>
+      <c r="N15" t="b">
+        <v>1</v>
+      </c>
+      <c r="O15" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="I15" t="s">
-        <v>86</v>
-      </c>
-      <c r="J15" s="38" t="s">
-        <v>87</v>
-      </c>
-      <c r="M15" t="b">
-        <v>1</v>
-      </c>
-      <c r="O15" s="48" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
+    </row>
+    <row r="16" ht="12" customHeight="1" spans="1:15">
       <c r="A16" s="1"/>
       <c r="D16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" t="s">
+        <v>87</v>
+      </c>
+      <c r="I16" t="s">
+        <v>88</v>
+      </c>
+      <c r="J16" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="E16" t="s">
+      <c r="M16" t="b">
+        <v>1</v>
+      </c>
+      <c r="N16" s="55" t="s">
+        <v>90</v>
+      </c>
+      <c r="O16" s="56" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" ht="13" customHeight="1" spans="4:15">
+      <c r="D17" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="F17" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" t="s">
+        <v>93</v>
+      </c>
+      <c r="I17" t="s">
+        <v>94</v>
+      </c>
+      <c r="J17" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="M17" t="b">
+        <v>1</v>
+      </c>
+      <c r="O17" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="I16" t="s">
-        <v>92</v>
-      </c>
-      <c r="J16" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="M16" t="b">
-        <v>1</v>
-      </c>
-      <c r="O16" s="12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15">
-      <c r="A17" s="1"/>
-      <c r="D17" t="s">
-        <v>95</v>
-      </c>
-      <c r="E17" t="s">
+    </row>
+    <row r="18" ht="13" customHeight="1" spans="4:15">
+      <c r="D18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" t="s">
         <v>19</v>
       </c>
-      <c r="H17" t="s">
-        <v>96</v>
-      </c>
-      <c r="I17" t="s">
+      <c r="H18" t="s">
         <v>97</v>
       </c>
-      <c r="J17" s="38" t="s">
+      <c r="I18" t="s">
         <v>98</v>
       </c>
-      <c r="M17" t="b">
-        <v>1</v>
-      </c>
-      <c r="O17" s="12" t="s">
+      <c r="J18" s="43" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="18" spans="1:15">
-      <c r="A18" s="1"/>
-      <c r="D18" t="s">
+      <c r="M18" t="b">
+        <v>1</v>
+      </c>
+      <c r="O18" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="E18" t="s">
-        <v>100</v>
-      </c>
-      <c r="H18" t="s">
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="1"/>
+      <c r="D19" t="s">
         <v>101</v>
       </c>
-      <c r="I18" t="s">
+      <c r="E19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="J18" s="40" t="s">
+      <c r="H19" t="s">
         <v>103</v>
       </c>
-      <c r="M18" s="5"/>
-      <c r="O18" s="12" t="s">
+      <c r="I19" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="19" s="25" customFormat="1" spans="1:17">
-      <c r="A19" s="30"/>
-      <c r="D19" s="25" t="s">
+      <c r="J19" s="43" t="s">
         <v>105</v>
       </c>
-      <c r="E19" s="25" t="s">
+      <c r="M19" t="b">
+        <v>1</v>
+      </c>
+      <c r="O19" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="1"/>
+      <c r="D20" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="I19" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="J19" s="25" t="s">
+      <c r="H20" t="s">
         <v>108</v>
       </c>
-      <c r="N19" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="O19" s="51"/>
-      <c r="Q19" s="25" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" s="26" customFormat="1" spans="1:15">
-      <c r="A20" s="31" t="s">
+      <c r="I20" t="s">
         <v>109</v>
       </c>
-      <c r="D20" s="26" t="s">
+      <c r="J20" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="E20" s="26" t="s">
+      <c r="M20" t="b">
+        <v>1</v>
+      </c>
+      <c r="O20" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="26" t="s">
+    </row>
+    <row r="21" s="25" customFormat="1" spans="1:17">
+      <c r="A21" s="32"/>
+      <c r="D21" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="I20" s="26" t="s">
+      <c r="E21" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" s="38"/>
+      <c r="H21" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="J20" s="41" t="s">
+      <c r="I21" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="J21" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="M21" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="N21" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="O21" s="57"/>
+      <c r="Q21" s="25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="1"/>
+      <c r="D22" t="s">
         <v>114</v>
       </c>
-      <c r="M20" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="N20" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="O20" s="52"/>
-    </row>
-    <row r="21" s="24" customFormat="1" spans="1:15">
-      <c r="A21" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="D21" s="24" t="s">
+      <c r="E22" t="s">
+        <v>114</v>
+      </c>
+      <c r="H22" t="s">
         <v>115</v>
       </c>
-      <c r="E21" s="24" t="s">
+      <c r="I22" t="s">
         <v>116</v>
       </c>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="24" t="s">
+      <c r="J22" s="45" t="s">
         <v>117</v>
       </c>
-      <c r="I21" s="24" t="s">
+      <c r="M22" s="58" t="b">
+        <v>1</v>
+      </c>
+      <c r="O22" s="59" t="s">
         <v>118</v>
       </c>
-      <c r="J21" s="39" t="s">
+    </row>
+    <row r="23" s="26" customFormat="1" spans="1:17">
+      <c r="A23" s="33"/>
+      <c r="D23" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="M21" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="N21" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="O21" s="42"/>
-    </row>
-    <row r="22" s="24" customFormat="1" spans="1:17">
-      <c r="A22" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="D22" s="24" t="s">
+      <c r="E23" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="E22" s="24" t="s">
+      <c r="I23" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="H22" s="24" t="s">
+      <c r="J23" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="I22" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="J22" s="39" t="s">
-        <v>122</v>
-      </c>
-      <c r="K22" s="42"/>
-      <c r="L22" s="42"/>
-      <c r="N22" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="24" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" s="27" customFormat="1" spans="1:17">
-      <c r="A23" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="D23" s="27" t="s">
+      <c r="N23" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="O23" s="60"/>
+      <c r="Q23" s="26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" s="27" customFormat="1" spans="1:15">
+      <c r="A24" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="E23" s="27" t="s">
+      <c r="D24" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="I24" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="J24" s="46" t="s">
+        <v>128</v>
+      </c>
+      <c r="M24" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="N24" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="O24" s="61"/>
+    </row>
+    <row r="25" s="28" customFormat="1" spans="1:15">
+      <c r="A25" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="E25" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="F25" s="41"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="I25" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="J25" s="47" t="s">
+        <v>133</v>
+      </c>
+      <c r="M25" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="N25" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="O25" s="48"/>
+    </row>
+    <row r="26" s="28" customFormat="1" spans="1:17">
+      <c r="A26" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="E26" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="H26" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="I26" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="J26" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="K26" s="48"/>
+      <c r="L26" s="48"/>
+      <c r="N26" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" s="29" customFormat="1" spans="1:17">
+      <c r="A27" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="E27" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="H23" s="27" t="s">
-        <v>124</v>
-      </c>
-      <c r="I23" s="27" t="s">
-        <v>124</v>
-      </c>
-      <c r="J23" s="39" t="s">
-        <v>124</v>
-      </c>
-      <c r="K23" s="43"/>
-      <c r="L23" s="43"/>
-      <c r="N23" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q23" s="27" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="1"/>
-      <c r="F24"/>
-      <c r="G24"/>
-      <c r="K24" s="44"/>
-      <c r="L24" s="44"/>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="1"/>
-      <c r="K25" s="44"/>
-      <c r="L25" s="44"/>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="1"/>
-      <c r="K26" s="44"/>
-      <c r="L26" s="44"/>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="1"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="12"/>
-    </row>
-    <row r="28" spans="1:1">
+      <c r="H27" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="I27" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="J27" s="47" t="s">
+        <v>138</v>
+      </c>
+      <c r="K27" s="49"/>
+      <c r="L27" s="49"/>
+      <c r="N27" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" s="1"/>
-    </row>
-    <row r="29" spans="1:1">
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="K28" s="50"/>
+      <c r="L28" s="50"/>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" s="1"/>
-    </row>
-    <row r="30" spans="1:1">
+      <c r="K29" s="50"/>
+      <c r="L29" s="50"/>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" s="1"/>
-    </row>
-    <row r="31" spans="1:1">
+      <c r="K30" s="50"/>
+      <c r="L30" s="50"/>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" s="1"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="1"/>
@@ -2659,11 +2900,24 @@
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="1"/>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="1"/>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="1"/>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="1"/>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.39375" footer="0.39375"/>
   <pageSetup paperSize="1" fitToWidth="0" pageOrder="overThenDown" orientation="portrait"/>
   <headerFooter/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2672,8 +2926,8 @@
   <sheetPr/>
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:B24"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.18095238095238" defaultRowHeight="12.75" outlineLevelCol="5"/>
@@ -2683,7 +2937,7 @@
     <col min="3" max="3" width="31.4571428571429" customWidth="1"/>
     <col min="4" max="4" width="37.6285714285714" customWidth="1"/>
     <col min="5" max="5" width="40.6285714285714" customWidth="1"/>
-    <col min="6" max="6" width="13.1809523809524" customWidth="1"/>
+    <col min="6" max="6" width="24.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2691,7 +2945,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -2708,53 +2962,53 @@
     </row>
     <row r="2" s="3" customFormat="1" spans="1:5">
       <c r="A2" s="6" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>126</v>
+        <v>140</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" s="3" customFormat="1" ht="15" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" s="3" customFormat="1" ht="15" customHeight="1" spans="1:6">
       <c r="A4" s="6" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="F4" s="3" t="b">
         <v>1</v>
@@ -2762,155 +3016,155 @@
     </row>
     <row r="5" s="3" customFormat="1" spans="1:5">
       <c r="A5" s="6" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" s="3" customFormat="1" spans="1:5">
       <c r="A6" s="6" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="C7" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="D7" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>149</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="C8" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="D8" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" s="4" customFormat="1" spans="1:5">
       <c r="A9" s="4" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" s="4" customFormat="1" spans="1:5">
       <c r="A10" s="4" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" s="4" customFormat="1" spans="1:5">
       <c r="A11" s="4" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" s="4" customFormat="1" spans="1:5">
       <c r="A12" s="4" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" s="5" customFormat="1" spans="1:6">
       <c r="A13" s="5" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="F13" s="5" t="b">
         <v>1</v>
@@ -2918,189 +3172,192 @@
     </row>
     <row r="14" s="5" customFormat="1" spans="1:5">
       <c r="A14" s="5" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" s="5" customFormat="1" spans="1:5">
       <c r="A15" s="5" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" s="5" customFormat="1" spans="1:5">
       <c r="A16" s="5" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17" s="5" customFormat="1" spans="1:5">
       <c r="A17" s="5" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="18" s="5" customFormat="1" spans="1:5">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" s="5" customFormat="1" spans="1:6">
       <c r="A18" s="5" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>193</v>
+        <v>207</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="19" s="5" customFormat="1" spans="1:5">
       <c r="A19" s="5" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>194</v>
+        <v>209</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>195</v>
+        <v>210</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>197</v>
+        <v>212</v>
       </c>
     </row>
     <row r="20" s="5" customFormat="1" spans="1:5">
       <c r="A20" s="5" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>198</v>
+        <v>213</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>199</v>
+        <v>214</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>200</v>
+        <v>215</v>
       </c>
     </row>
     <row r="21" s="4" customFormat="1" spans="1:5">
       <c r="A21" s="4" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>203</v>
+        <v>218</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
     </row>
     <row r="22" s="4" customFormat="1" spans="1:5">
       <c r="A22" s="4" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>206</v>
+        <v>221</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>208</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23" s="4" customFormat="1" spans="1:5">
       <c r="A23" s="4" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>210</v>
+        <v>225</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>211</v>
+        <v>226</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>212</v>
+        <v>227</v>
       </c>
     </row>
     <row r="24" s="4" customFormat="1" spans="1:5">
       <c r="A24" s="4" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>214</v>
+        <v>229</v>
       </c>
     </row>
     <row r="25" s="4" customFormat="1" spans="2:2">
@@ -3131,30 +3388,30 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="C1" t="s">
-        <v>217</v>
+        <v>232</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>218</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>219</v>
+        <v>234</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="C2" t="s">
-        <v>221</v>
+        <v>236</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>222</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>